<commit_message>
appoint1:adjusting and updating the appoitment form
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
   <si>
     <t>type</t>
   </si>
@@ -147,7 +147,13 @@
     <t>type_appoint</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>Appointment Type</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Any notes about this Appointment?</t>
   </si>
   <si>
     <t>select_one lab or_other</t>
@@ -166,15 +172,6 @@
   </si>
   <si>
     <t>Date of Appointment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date </t>
-  </si>
-  <si>
-    <t>date_reminder</t>
-  </si>
-  <si>
-    <t>Is there a specific date where you would like to be reminded of this appointment?</t>
   </si>
   <si>
     <t>list_name</t>
@@ -634,6 +631,7 @@
     <col customWidth="1" min="1" max="1" width="19.75"/>
     <col customWidth="1" min="3" max="3" width="59.88"/>
     <col customWidth="1" min="4" max="4" width="24.38"/>
+    <col customWidth="1" min="7" max="7" width="33.5"/>
     <col customWidth="1" min="9" max="9" width="19.63"/>
   </cols>
   <sheetData>
@@ -1030,38 +1028,38 @@
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="27">
@@ -1089,7 +1087,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1103,10 +1101,10 @@
         <v>37</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3">
@@ -1114,10 +1112,10 @@
         <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
@@ -1125,10 +1123,10 @@
         <v>37</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -1136,10 +1134,10 @@
         <v>37</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
@@ -1147,10 +1145,10 @@
         <v>37</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7">
@@ -1158,32 +1156,32 @@
         <v>37</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1206,47 +1204,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>78</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>79</v>
       </c>
       <c r="C2" s="15" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-06-29_11-21</v>
+        <v>2022-07-13_10-15</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>80</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>81</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
appoint1:changing the appointment form to schedule appointment
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="81">
   <si>
     <t>type</t>
   </si>
@@ -51,7 +51,7 @@
     <t>inputs</t>
   </si>
   <si>
-    <t xml:space="preserve"> Appointment Form</t>
+    <t xml:space="preserve"> Schedule Appointment </t>
   </si>
   <si>
     <t>./source = 'user'</t>
@@ -247,9 +247,6 @@
   </si>
   <si>
     <t>default_language</t>
-  </si>
-  <si>
-    <t>Appointment Form</t>
   </si>
   <si>
     <t>appointment</t>
@@ -1227,24 +1224,24 @@
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>77</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>78</v>
       </c>
       <c r="C2" s="15" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-13_10-15</v>
+        <v>2022-07-14_15-01</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>80</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:updating the appointment and lab forms
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -183,14 +183,14 @@
     <t>Clinical Appointment</t>
   </si>
   <si>
-    <t>social</t>
+    <t>social worker</t>
   </si>
   <si>
     <t xml:space="preserve">Social Worker Appointment
 </t>
   </si>
   <si>
-    <t>case</t>
+    <t>case manager</t>
   </si>
   <si>
     <t xml:space="preserve">Case Manager Appointment
@@ -201,13 +201,13 @@
 </t>
   </si>
   <si>
-    <t>internal</t>
+    <t xml:space="preserve">internal </t>
   </si>
   <si>
     <t xml:space="preserve">Internal Referral </t>
   </si>
   <si>
-    <t>external</t>
+    <t xml:space="preserve">external </t>
   </si>
   <si>
     <t xml:space="preserve">External Referral </t>
@@ -216,13 +216,13 @@
     <t>lab</t>
   </si>
   <si>
-    <t>count</t>
+    <t>cd4 count</t>
   </si>
   <si>
     <t>CD4 count</t>
   </si>
   <si>
-    <t>load</t>
+    <t xml:space="preserve">viral load </t>
   </si>
   <si>
     <t>Viral Load</t>
@@ -1079,6 +1079,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="2" max="2" width="23.88"/>
     <col customWidth="1" min="3" max="3" width="23.25"/>
   </cols>
   <sheetData>
@@ -1231,7 +1232,7 @@
       </c>
       <c r="C2" s="15" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-21_20-25</v>
+        <v>2022-07-26_09-57</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
auto:adding more skip logic to the viral load lab test result form and changing the choices in the appointment form
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
   <si>
     <t>type</t>
   </si>
@@ -177,37 +177,40 @@
     <t>list_name</t>
   </si>
   <si>
-    <t>clinical</t>
+    <t>clinical appointment</t>
   </si>
   <si>
     <t>Clinical Appointment</t>
   </si>
   <si>
-    <t>social worker</t>
+    <t>social worker appointment</t>
   </si>
   <si>
     <t xml:space="preserve">Social Worker Appointment
 </t>
   </si>
   <si>
-    <t>case manager</t>
+    <t xml:space="preserve">case manager appointment </t>
   </si>
   <si>
     <t xml:space="preserve">Case Manager Appointment
 </t>
   </si>
   <si>
+    <t>lab test appointment</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lab Test Appointment
 </t>
   </si>
   <si>
-    <t xml:space="preserve">internal </t>
+    <t>internal referral</t>
   </si>
   <si>
     <t xml:space="preserve">Internal Referral </t>
   </si>
   <si>
-    <t xml:space="preserve">external </t>
+    <t>external referral</t>
   </si>
   <si>
     <t xml:space="preserve">External Referral </t>
@@ -1132,10 +1135,10 @@
         <v>37</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -1143,10 +1146,10 @@
         <v>37</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
@@ -1154,32 +1157,32 @@
         <v>37</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1202,25 +1205,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
@@ -1228,21 +1231,21 @@
         <v>12</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" s="15" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-26_09-57</v>
+        <v>2022-07-26_12-16</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:adding isFormArraySubmittedInWindow in nools-extras plus more chages in app forms
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -165,7 +165,7 @@
     <t>Lab test:</t>
   </si>
   <si>
-    <t>${type_appoint} = 'lab_test'</t>
+    <t>${type_appoint} = 'lab test appointment'</t>
   </si>
   <si>
     <t>date_appoint</t>
@@ -630,7 +630,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="19.75"/>
     <col customWidth="1" min="3" max="3" width="59.88"/>
-    <col customWidth="1" min="4" max="4" width="24.38"/>
+    <col customWidth="1" min="4" max="4" width="36.75"/>
     <col customWidth="1" min="7" max="7" width="33.5"/>
     <col customWidth="1" min="9" max="9" width="19.63"/>
   </cols>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="C2" s="15" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-26_12-16</v>
+        <v>2022-07-26_16-56</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
auto:updating the appoitment form with new changes
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
   <si>
     <t>type</t>
   </si>
@@ -129,43 +129,40 @@
     <t>appoint</t>
   </si>
   <si>
+    <t>select_one appoint</t>
+  </si>
+  <si>
+    <t>type_appoint</t>
+  </si>
+  <si>
+    <t>Appointment Type</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Any notes about this Appointment?</t>
+  </si>
+  <si>
+    <t>select_one lab or_other</t>
+  </si>
+  <si>
+    <t>lab_test</t>
+  </si>
+  <si>
+    <t>Blood Draw:</t>
+  </si>
+  <si>
+    <t>${type_appoint} = 'lab test appointment'</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
-    <t>enter</t>
-  </si>
-  <si>
-    <t>Date Entered</t>
-  </si>
-  <si>
-    <t>today()</t>
-  </si>
-  <si>
-    <t>select_one appoint</t>
-  </si>
-  <si>
-    <t>type_appoint</t>
-  </si>
-  <si>
-    <t>Appointment Type</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>Any notes about this Appointment?</t>
-  </si>
-  <si>
-    <t>select_one lab or_other</t>
-  </si>
-  <si>
-    <t>lab_test</t>
-  </si>
-  <si>
-    <t>Lab test:</t>
-  </si>
-  <si>
-    <t>${type_appoint} = 'lab test appointment'</t>
+    <t>date_appoint1</t>
+  </si>
+  <si>
+    <t>Date of Expected Blood Draw</t>
   </si>
   <si>
     <t>date_appoint</t>
@@ -197,10 +194,10 @@
 </t>
   </si>
   <si>
-    <t>lab test appointment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lab Test Appointment
+    <t>blood draw appointment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blood Draw Appointment
 </t>
   </si>
   <si>
@@ -1008,32 +1005,29 @@
       <c r="C22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J22" s="6" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="D24" s="12" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1047,19 +1041,17 @@
       <c r="C25" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="D25" s="12"/>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27">
@@ -1088,7 +1080,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1102,10 +1094,10 @@
         <v>37</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3">
@@ -1113,10 +1105,10 @@
         <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
@@ -1124,10 +1116,10 @@
         <v>37</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5">
@@ -1135,10 +1127,10 @@
         <v>37</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -1146,10 +1138,10 @@
         <v>37</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7">
@@ -1157,32 +1149,32 @@
         <v>37</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1205,25 +1197,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2">
@@ -1231,21 +1223,21 @@
         <v>12</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="15" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-26_16-56</v>
+        <v>2022-08-02_10-05</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>80</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:adding skip logic to the appointment form when the blood draw appointment is selected
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -153,7 +153,7 @@
     <t>Blood Draw:</t>
   </si>
   <si>
-    <t>${type_appoint} = 'lab test appointment'</t>
+    <t>${type_appoint} = 'blood draw appointment'</t>
   </si>
   <si>
     <t>date</t>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="C2" s="15" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-08-02_10-05</v>
+        <v>2022-08-03_15-02</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
auto:adding an image in the schedule appoitment form
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="86">
   <si>
     <t>type</t>
   </si>
@@ -24,9 +24,15 @@
     <t>label</t>
   </si>
   <si>
+    <t>media::image::en</t>
+  </si>
+  <si>
     <t>relevant</t>
   </si>
   <si>
+    <t>parameters</t>
+  </si>
+  <si>
     <t>appearance</t>
   </si>
   <si>
@@ -138,10 +144,19 @@
     <t>Appointment Type</t>
   </si>
   <si>
-    <t>notes</t>
+    <t>note</t>
+  </si>
+  <si>
+    <t>welcome</t>
   </si>
   <si>
     <t>Any notes about this Appointment?</t>
+  </si>
+  <si>
+    <t>image.png</t>
+  </si>
+  <si>
+    <t>h1 blue</t>
   </si>
   <si>
     <t>select_one lab or_other</t>
@@ -349,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -358,6 +373,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -626,10 +644,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="19.75"/>
-    <col customWidth="1" min="3" max="3" width="59.88"/>
-    <col customWidth="1" min="4" max="4" width="36.75"/>
-    <col customWidth="1" min="7" max="7" width="33.5"/>
-    <col customWidth="1" min="9" max="9" width="19.63"/>
+    <col customWidth="1" min="3" max="4" width="59.88"/>
+    <col customWidth="1" min="5" max="6" width="36.75"/>
+    <col customWidth="1" min="9" max="9" width="33.5"/>
+    <col customWidth="1" min="11" max="11" width="19.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -642,421 +660,479 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1080,7 +1156,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1090,91 +1166,91 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>54</v>
+      <c r="A2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>56</v>
+      <c r="A3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>58</v>
+      <c r="A4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>60</v>
+      <c r="A5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>62</v>
+      <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>64</v>
+      <c r="A7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>67</v>
+      <c r="A8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>69</v>
+      <c r="A9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1197,47 +1273,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="15" t="str">
+      <c r="A2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="16" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-08-03_15-02</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16" t="s">
-        <v>80</v>
+        <v>2022-08-04_12-00</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:including Psychologist Appointment and Adherence Counselor Appointment to the appointment form
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
   <si>
     <t>type</t>
   </si>
@@ -214,6 +214,18 @@
   <si>
     <t xml:space="preserve">Blood Draw Appointment
 </t>
+  </si>
+  <si>
+    <t>psychologist appointment</t>
+  </si>
+  <si>
+    <t>Psychologist Appointment</t>
+  </si>
+  <si>
+    <t>adherence counselor appointment</t>
+  </si>
+  <si>
+    <t>Adherence Counselor Appointment</t>
   </si>
   <si>
     <t>internal referral</t>
@@ -1150,8 +1162,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="23.88"/>
-    <col customWidth="1" min="3" max="3" width="23.25"/>
+    <col customWidth="1" min="2" max="2" width="36.25"/>
+    <col customWidth="1" min="3" max="3" width="38.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1233,24 +1245,46 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="7" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
         <v>74</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1273,25 +1307,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2">
@@ -1299,21 +1333,21 @@
         <v>14</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C2" s="16" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-08-04_12-00</v>
+        <v>2022-08-10_11-27</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:updating the skip logic in  schedule appointment form
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
   <si>
     <t>type</t>
   </si>
@@ -144,46 +144,52 @@
     <t>Appointment Type</t>
   </si>
   <si>
+    <t>welcome</t>
+  </si>
+  <si>
+    <t>Any notes about this Appointment?</t>
+  </si>
+  <si>
+    <t>h1 blue</t>
+  </si>
+  <si>
+    <t>select_one lab or_other</t>
+  </si>
+  <si>
+    <t>lab_test</t>
+  </si>
+  <si>
+    <t>Blood Draw:</t>
+  </si>
+  <si>
+    <t>${type_appoint} = 'blood draw appointment'</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>date_appoint</t>
+  </si>
+  <si>
+    <t>Date of Appointment</t>
+  </si>
+  <si>
     <t>note</t>
   </si>
   <si>
-    <t>welcome</t>
-  </si>
-  <si>
-    <t>Any notes about this Appointment?</t>
+    <t>image1</t>
+  </si>
+  <si>
+    <t>Image</t>
   </si>
   <si>
     <t>image.png</t>
   </si>
   <si>
-    <t>h1 blue</t>
-  </si>
-  <si>
-    <t>select_one lab or_other</t>
-  </si>
-  <si>
-    <t>lab_test</t>
-  </si>
-  <si>
-    <t>Blood Draw:</t>
-  </si>
-  <si>
-    <t>${type_appoint} = 'blood draw appointment'</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>date_appoint1</t>
   </si>
   <si>
     <t>Date of Expected Blood Draw</t>
-  </si>
-  <si>
-    <t>date_appoint</t>
-  </si>
-  <si>
-    <t>Date of Appointment</t>
   </si>
   <si>
     <t>list_name</t>
@@ -1085,65 +1091,80 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7"/>
+      <c r="G23" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F24" s="13"/>
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="D25" s="7"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="E26" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1168,7 +1189,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1182,10 +1203,10 @@
         <v>39</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3">
@@ -1193,10 +1214,10 @@
         <v>39</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
@@ -1204,10 +1225,10 @@
         <v>39</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5">
@@ -1215,10 +1236,10 @@
         <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6">
@@ -1226,10 +1247,10 @@
         <v>39</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7">
@@ -1237,10 +1258,10 @@
         <v>39</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8">
@@ -1248,10 +1269,10 @@
         <v>39</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9">
@@ -1259,32 +1280,32 @@
         <v>39</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1307,25 +1328,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
@@ -1333,21 +1354,21 @@
         <v>14</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="16" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-08-10_11-27</v>
+        <v>2022-08-11_11-07</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:Make sure the  Date of Expected Blood draw only appears when the provider has selected Blood draw appointment
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="92">
   <si>
     <t>type</t>
   </si>
@@ -662,9 +662,11 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="19.75"/>
-    <col customWidth="1" min="3" max="4" width="59.88"/>
-    <col customWidth="1" min="5" max="6" width="36.75"/>
-    <col customWidth="1" min="9" max="9" width="33.5"/>
+    <col customWidth="1" min="3" max="3" width="27.38"/>
+    <col customWidth="1" min="4" max="4" width="15.88"/>
+    <col customWidth="1" min="5" max="5" width="36.75"/>
+    <col customWidth="1" min="6" max="6" width="11.88"/>
+    <col customWidth="1" min="9" max="9" width="22.63"/>
     <col customWidth="1" min="11" max="11" width="19.63"/>
   </cols>
   <sheetData>
@@ -1160,7 +1162,9 @@
         <v>58</v>
       </c>
       <c r="D27" s="7"/>
-      <c r="E27" s="13"/>
+      <c r="E27" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="F27" s="13"/>
     </row>
     <row r="28">
@@ -1358,7 +1362,7 @@
       </c>
       <c r="C2" s="16" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-08-11_11-07</v>
+        <v>2022-10-19_11-28</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
auto:Making sure date of appointment doesn't show when person selects Blood draw
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
   <si>
     <t>type</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Date of Appointment</t>
+  </si>
+  <si>
+    <t>${type_appoint} != 'blood draw appointment'</t>
   </si>
   <si>
     <t>note</t>
@@ -1133,19 +1136,22 @@
         <v>52</v>
       </c>
       <c r="D25" s="7"/>
+      <c r="E25" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>49</v>
@@ -1156,10 +1162,10 @@
         <v>50</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="13" t="s">
@@ -1193,7 +1199,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1207,10 +1213,10 @@
         <v>39</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3">
@@ -1218,10 +1224,10 @@
         <v>39</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
@@ -1229,10 +1235,10 @@
         <v>39</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
@@ -1240,10 +1246,10 @@
         <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6">
@@ -1251,10 +1257,10 @@
         <v>39</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
@@ -1262,10 +1268,10 @@
         <v>39</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8">
@@ -1273,10 +1279,10 @@
         <v>39</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9">
@@ -1284,32 +1290,32 @@
         <v>39</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1332,25 +1338,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
@@ -1358,21 +1364,21 @@
         <v>14</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" s="16" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-10-19_11-28</v>
+        <v>2022-10-24_14-02</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:changing the appointment form for reflect data from the enrollment form
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="128">
   <si>
     <t>type</t>
   </si>
@@ -105,6 +105,18 @@
     <t>sex</t>
   </si>
   <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>aka</t>
+  </si>
+  <si>
+    <t>tsis</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
@@ -132,9 +144,106 @@
     <t>../inputs/contact/name</t>
   </si>
   <si>
+    <t>patient_name1</t>
+  </si>
+  <si>
+    <t>../inputs/contact/name1</t>
+  </si>
+  <si>
+    <t>patient_aka</t>
+  </si>
+  <si>
+    <t>../inputs/contact/aka</t>
+  </si>
+  <si>
+    <t>patient_tsis</t>
+  </si>
+  <si>
+    <t>../inputs/contact/tsis</t>
+  </si>
+  <si>
+    <t>patient_at</t>
+  </si>
+  <si>
+    <t>../inputs/contact/at</t>
+  </si>
+  <si>
+    <t>patient_date_of_birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of birth </t>
+  </si>
+  <si>
+    <t>../inputs/contact/date_of_birth</t>
+  </si>
+  <si>
+    <t>fast_name_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/fstname != '', instance('contact-summary')/context/fstname, .)</t>
+  </si>
+  <si>
+    <t>last_name_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/lstname != '', instance('contact-summary')/context/lstname, .)</t>
+  </si>
+  <si>
+    <t>date_of_birth_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_date_of_birth != '', instance('contact-summary')/context/patient_date_of_birth, .)</t>
+  </si>
+  <si>
+    <t>aka_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_aka != '', instance('contact-summary')/context/patient_aka, .)</t>
+  </si>
+  <si>
+    <t>tsis_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_tsis != '', instance('contact-summary')/context/patient_tsis, .)</t>
+  </si>
+  <si>
+    <t>at_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_at != '', instance('contact-summary')/context/patient_at, .)</t>
+  </si>
+  <si>
+    <t>yr_date_of_birth_ctx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int(int(format-date(today(), "%Y") - format-date(${date_of_birth_ctx}, "%Y")) )
+</t>
+  </si>
+  <si>
     <t>appoint</t>
   </si>
   <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}  ${last_name_ctx}**&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>${aka_ctx}  |  ${yr_date_of_birth_ctx} yr   ${at_ctx}</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>${tsis_ctx}</t>
+  </si>
+  <si>
     <t>select_one appoint</t>
   </si>
   <si>
@@ -175,9 +284,6 @@
   </si>
   <si>
     <t>${type_appoint} != 'blood draw appointment'</t>
-  </si>
-  <si>
-    <t>note</t>
   </si>
   <si>
     <t>image1</t>
@@ -385,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -422,8 +528,14 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -665,10 +777,12 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="19.75"/>
-    <col customWidth="1" min="3" max="3" width="27.38"/>
-    <col customWidth="1" min="4" max="4" width="15.88"/>
+    <col customWidth="1" min="3" max="3" width="62.13"/>
+    <col customWidth="1" min="4" max="4" width="29.0"/>
     <col customWidth="1" min="5" max="5" width="36.75"/>
     <col customWidth="1" min="6" max="6" width="11.88"/>
+    <col customWidth="1" min="7" max="7" width="29.0"/>
+    <col customWidth="1" min="8" max="8" width="15.25"/>
     <col customWidth="1" min="9" max="9" width="22.63"/>
     <col customWidth="1" min="11" max="11" width="19.63"/>
   </cols>
@@ -874,7 +988,6 @@
         <v>19</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
         <v>17</v>
@@ -883,83 +996,155 @@
       <c r="I10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
+        <v>12</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="D15" s="10"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -969,10 +1154,14 @@
     </row>
     <row r="16">
       <c r="A16" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
+        <v>12</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="D16" s="10"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -981,201 +1170,589 @@
       <c r="I16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
+      <c r="A17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="D17" s="10"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="D18" s="10"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
     <row r="19">
       <c r="A19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>34</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="I19" s="4"/>
     </row>
     <row r="20">
       <c r="A20" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="I20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="4"/>
+      <c r="A21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="4"/>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C24" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D24" s="10"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="7" t="s">
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4"/>
+      <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
+      <c r="Z38" s="4"/>
+      <c r="AA38" s="4"/>
+      <c r="AB38" s="4"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="4"/>
+      <c r="AA39" s="4"/>
+      <c r="AB39" s="4"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+      <c r="W40" s="4"/>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4"/>
+      <c r="Z40" s="4"/>
+      <c r="AA40" s="4"/>
+      <c r="AB40" s="4"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" s="7"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="G23" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" s="13"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" s="13"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="7" t="s">
-        <v>32</v>
+      <c r="B42" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="G42" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F43" s="15"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F46" s="15"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1199,7 +1776,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1210,112 +1787,112 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1338,47 +1915,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>88</v>
+        <v>122</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="16" t="str">
+      <c r="B2" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="18" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-10-24_14-02</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17" t="s">
-        <v>92</v>
+        <v>2023-06-21_21-29</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:updating patient identifier card on the appointment form
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="138">
   <si>
     <t>type</t>
   </si>
@@ -117,6 +117,9 @@
     <t>at</t>
   </si>
   <si>
+    <t>genda</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
@@ -160,6 +163,12 @@
   </si>
   <si>
     <t>../inputs/contact/tsis</t>
+  </si>
+  <si>
+    <t>patient_genda</t>
+  </si>
+  <si>
+    <t>../inputs/contact/genda</t>
   </si>
   <si>
     <t>patient_at</t>
@@ -220,6 +229,12 @@
 </t>
   </si>
   <si>
+    <t>gender_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_genda != '', instance('contact-summary')/context/patient_genda, .)</t>
+  </si>
+  <si>
     <t>appoint</t>
   </si>
   <si>
@@ -232,16 +247,31 @@
     <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}  ${last_name_ctx}**&lt;/i&gt;</t>
   </si>
   <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>${aka_ctx}  |  ${yr_date_of_birth_ctx} yr   ${at_ctx}</t>
+    <t xml:space="preserve">h1 yellow </t>
+  </si>
+  <si>
+    <t>nick</t>
+  </si>
+  <si>
+    <t>Nickname: **${aka_ctx}**</t>
+  </si>
+  <si>
+    <t>age_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age: **${yr_date_of_birth_ctx} yr**  </t>
+  </si>
+  <si>
+    <t>gender_n</t>
+  </si>
+  <si>
+    <t>Gender Identity: **${gender_ctx}**</t>
   </si>
   <si>
     <t>dob</t>
   </si>
   <si>
-    <t>${tsis_ctx}</t>
+    <t>TSIS: **${tsis_ctx}**</t>
   </si>
   <si>
     <t>select_one appoint</t>
@@ -491,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -529,6 +559,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -781,7 +814,7 @@
     <col customWidth="1" min="4" max="4" width="29.0"/>
     <col customWidth="1" min="5" max="5" width="36.75"/>
     <col customWidth="1" min="6" max="6" width="11.88"/>
-    <col customWidth="1" min="7" max="7" width="29.0"/>
+    <col customWidth="1" min="7" max="7" width="42.13"/>
     <col customWidth="1" min="8" max="8" width="15.25"/>
     <col customWidth="1" min="9" max="9" width="22.63"/>
     <col customWidth="1" min="11" max="11" width="19.63"/>
@@ -1136,28 +1169,47 @@
       <c r="Z14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="10"/>
+      <c r="C15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
     </row>
     <row r="16">
       <c r="A16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>19</v>
@@ -1170,11 +1222,11 @@
       <c r="I16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>35</v>
+      <c r="A17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>19</v>
@@ -1182,9 +1234,7 @@
       <c r="D17" s="10"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
@@ -1193,7 +1243,7 @@
         <v>26</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>19</v>
@@ -1208,21 +1258,27 @@
       <c r="I18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="D19" s="10"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20">
       <c r="A20" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
@@ -1235,7 +1291,7 @@
     </row>
     <row r="21">
       <c r="A21" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
@@ -1248,7 +1304,7 @@
     </row>
     <row r="22">
       <c r="A22" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
@@ -1263,30 +1319,24 @@
       <c r="A23" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="I23" s="4"/>
     </row>
     <row r="24">
       <c r="A24" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="4"/>
@@ -1294,33 +1344,34 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="4"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="4" t="s">
-        <v>44</v>
+      <c r="I25" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>19</v>
@@ -1330,15 +1381,15 @@
       <c r="F26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>19</v>
@@ -1348,15 +1399,15 @@
       <c r="F27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>19</v>
@@ -1366,33 +1417,51 @@
       <c r="F28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="I29" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>19</v>
@@ -1402,33 +1471,33 @@
       <c r="F30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>19</v>
@@ -1437,16 +1506,16 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="12" t="s">
-        <v>59</v>
+      <c r="I32" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>19</v>
@@ -1456,15 +1525,15 @@
       <c r="F33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>19</v>
@@ -1473,16 +1542,16 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="4" t="s">
-        <v>63</v>
+      <c r="I34" s="12" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>19</v>
@@ -1492,15 +1561,15 @@
       <c r="F35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>19</v>
@@ -1510,15 +1579,15 @@
       <c r="F36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>19</v>
@@ -1526,83 +1595,47 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
-      <c r="AA37" s="4"/>
-      <c r="AB37" s="4"/>
+      <c r="I37" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="14" t="s">
-        <v>70</v>
-      </c>
       <c r="C38" s="4" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-      <c r="T38" s="4"/>
-      <c r="U38" s="4"/>
-      <c r="V38" s="4"/>
-      <c r="W38" s="4"/>
-      <c r="X38" s="4"/>
-      <c r="Y38" s="4"/>
-      <c r="Z38" s="4"/>
-      <c r="AA38" s="4"/>
-      <c r="AB38" s="4"/>
+      <c r="I38" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>72</v>
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="G39" s="13"/>
       <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
+      <c r="I39" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
@@ -1620,23 +1653,23 @@
       <c r="X39" s="4"/>
       <c r="Y39" s="4"/>
       <c r="Z39" s="4"/>
-      <c r="AA39" s="4"/>
-      <c r="AB39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="s">
-        <v>69</v>
+      <c r="A40" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="G40" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -1660,99 +1693,281 @@
       <c r="AB40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
+      <c r="Z41" s="4"/>
+      <c r="AA41" s="4"/>
+      <c r="AB41" s="4"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="7" t="s">
+      <c r="C42" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="4"/>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4"/>
+      <c r="AB42" s="4"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="G42" s="7" t="s">
+      <c r="C43" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="7" t="s">
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4"/>
+      <c r="AB43" s="4"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="C44" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="4"/>
+      <c r="Y44" s="4"/>
+      <c r="Z44" s="4"/>
+      <c r="AA44" s="4"/>
+      <c r="AB44" s="4"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="15" t="s">
+      <c r="C45" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F43" s="15"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
+      <c r="AA45" s="4"/>
+      <c r="AB45" s="4"/>
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D46" s="7"/>
-      <c r="E46" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F46" s="15"/>
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="G47" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F48" s="16"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" s="7"/>
+      <c r="E51" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F51" s="16"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1776,7 +1991,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1787,112 +2002,112 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1915,47 +2130,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>123</v>
+        <v>132</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="18" t="str">
+      <c r="B2" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="19" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-06-21_21-29</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19" t="s">
-        <v>127</v>
+        <v>2023-07-31_20-57</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:updating app forms with new styling
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="140">
   <si>
     <t>type</t>
   </si>
@@ -238,16 +238,16 @@
     <t>appoint</t>
   </si>
   <si>
+    <t>field-list summary</t>
+  </si>
+  <si>
     <t>note</t>
   </si>
   <si>
     <t>first_name</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}  ${last_name_ctx}**&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h1 yellow </t>
+    <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}**&lt;/i&gt;</t>
   </si>
   <si>
     <t>nick</t>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>TSIS: **${tsis_ctx}**</t>
+  </si>
+  <si>
+    <t>n_special_instruction_title</t>
+  </si>
+  <si>
+    <t>h1 yellow</t>
   </si>
   <si>
     <t>select_one appoint</t>
@@ -437,7 +443,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -471,6 +477,16 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="8.0"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
@@ -481,7 +497,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -498,6 +514,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE5CD"/>
+        <bgColor rgb="FFFCE5CD"/>
       </patternFill>
     </fill>
   </fills>
@@ -521,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -570,19 +592,28 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1667,8 +1698,8 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="4" t="s">
-        <v>16</v>
+      <c r="G40" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
@@ -1694,20 +1725,18 @@
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="4" t="s">
         <v>76</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="8" t="s">
-        <v>77</v>
-      </c>
+      <c r="G41" s="8"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -1732,7 +1761,7 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>78</v>
@@ -1768,7 +1797,7 @@
     </row>
     <row r="43">
       <c r="A43" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>80</v>
@@ -1804,7 +1833,7 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>82</v>
@@ -1840,7 +1869,7 @@
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>84</v>
@@ -1875,20 +1904,46 @@
       <c r="AB45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="C46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="7"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="4"/>
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>89</v>
@@ -1897,80 +1952,97 @@
         <v>90</v>
       </c>
       <c r="D47" s="7"/>
-      <c r="G47" s="7" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="D48" s="7"/>
+      <c r="G48" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F48" s="16"/>
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="D49" s="7"/>
+      <c r="E49" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7" t="s">
-        <v>99</v>
-      </c>
+      <c r="F49" s="19"/>
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B50" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="D50" s="7"/>
+      <c r="E50" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F51" s="16"/>
+      <c r="E51" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F52" s="19"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="7" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="D46">
+      <formula1>"yes,no"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1991,7 +2063,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2005,10 +2077,10 @@
         <v>73</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3">
@@ -2016,10 +2088,10 @@
         <v>73</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
@@ -2027,10 +2099,10 @@
         <v>73</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
@@ -2038,10 +2110,10 @@
         <v>73</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6">
@@ -2049,10 +2121,10 @@
         <v>73</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7">
@@ -2060,10 +2132,10 @@
         <v>73</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8">
@@ -2071,10 +2143,10 @@
         <v>73</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9">
@@ -2082,32 +2154,32 @@
         <v>73</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2130,47 +2202,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="19" t="str">
+      <c r="B2" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="22" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-07-31_20-57</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
+        <v>2023-08-03_21-27</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>137</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto: Update the Appointment Form ie added one field, changed wording of one question, made some fields required and removing the image from the form
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="139">
   <si>
     <t>type</t>
   </si>
@@ -280,6 +280,16 @@
     <t>h1 yellow</t>
   </si>
   <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of Person Completing form
+</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>select_one appoint</t>
   </si>
   <si>
@@ -292,10 +302,7 @@
     <t>welcome</t>
   </si>
   <si>
-    <t>Any notes about this Appointment?</t>
-  </si>
-  <si>
-    <t>h1 blue</t>
+    <t>Notes about this Appointment?</t>
   </si>
   <si>
     <t>select_one lab or_other</t>
@@ -320,15 +327,6 @@
   </si>
   <si>
     <t>${type_appoint} != 'blood draw appointment'</t>
-  </si>
-  <si>
-    <t>image1</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>image.png</t>
   </si>
   <si>
     <t>date_appoint1</t>
@@ -543,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -600,6 +598,12 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1942,95 +1946,126 @@
       <c r="AB46" s="4"/>
     </row>
     <row r="47">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="C47" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="5"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D47" s="7"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="4"/>
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D48" s="7"/>
-      <c r="G48" s="7" t="s">
-        <v>93</v>
+      <c r="H48" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="C49" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D49" s="7"/>
-      <c r="E49" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F49" s="19"/>
+      <c r="G49" s="7"/>
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="D50" s="7"/>
+      <c r="E50" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C50" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7" t="s">
-        <v>101</v>
+      <c r="F50" s="21"/>
+      <c r="H50" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="7"/>
+      <c r="E51" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>97</v>
+      <c r="H51" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="D52" s="7"/>
-      <c r="E52" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F52" s="19"/>
+      <c r="E52" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F52" s="21"/>
+      <c r="H52" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="7" t="s">
@@ -2039,7 +2074,7 @@
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D46">
+    <dataValidation type="list" allowBlank="1" sqref="D46:D47">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2063,7 +2098,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2077,10 +2112,10 @@
         <v>73</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3">
@@ -2088,10 +2123,10 @@
         <v>73</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
@@ -2099,10 +2134,10 @@
         <v>73</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="5">
@@ -2110,10 +2145,10 @@
         <v>73</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="6">
@@ -2121,10 +2156,10 @@
         <v>73</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="7">
@@ -2132,10 +2167,10 @@
         <v>73</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="8">
@@ -2143,10 +2178,10 @@
         <v>73</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="9">
@@ -2154,32 +2189,32 @@
         <v>73</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>125</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2202,47 +2237,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="20" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="24" t="str">
+        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
+        <v>2023-08-20_11-19</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="22" t="str">
-        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-08-03_21-27</v>
-      </c>
-      <c r="D2" s="23" t="s">
+      <c r="E2" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="F2" s="25"/>
+      <c r="G2" s="25" t="s">
         <v>138</v>
-      </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:removing some labels from the patient card
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="136">
   <si>
     <t>type</t>
   </si>
@@ -250,22 +250,10 @@
     <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}**&lt;/i&gt;</t>
   </si>
   <si>
-    <t>nick</t>
-  </si>
-  <si>
-    <t>Nickname: **${aka_ctx}**</t>
-  </si>
-  <si>
     <t>age_n</t>
   </si>
   <si>
     <t xml:space="preserve">Age: **${yr_date_of_birth_ctx} yr**  </t>
-  </si>
-  <si>
-    <t>gender_n</t>
-  </si>
-  <si>
-    <t>Gender Identity: **${gender_ctx}**</t>
   </si>
   <si>
     <t>dob</t>
@@ -423,6 +411,9 @@
   </si>
   <si>
     <t>default_language</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Appointment </t>
   </si>
   <si>
     <t>appointment</t>
@@ -845,6 +836,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="19.75"/>
+    <col customWidth="1" min="2" max="2" width="29.5"/>
     <col customWidth="1" min="3" max="3" width="62.13"/>
     <col customWidth="1" min="4" max="4" width="29.0"/>
     <col customWidth="1" min="5" max="5" width="36.75"/>
@@ -1836,245 +1828,173 @@
       <c r="AB43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="17" t="s">
         <v>82</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-      <c r="T44" s="4"/>
-      <c r="U44" s="4"/>
-      <c r="V44" s="4"/>
-      <c r="W44" s="4"/>
-      <c r="X44" s="4"/>
-      <c r="Y44" s="4"/>
-      <c r="Z44" s="4"/>
-      <c r="AA44" s="4"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="5"/>
+      <c r="AA44" s="5"/>
       <c r="AB44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="15" t="s">
+      <c r="A45" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
-      <c r="T45" s="4"/>
-      <c r="U45" s="4"/>
-      <c r="V45" s="4"/>
-      <c r="W45" s="4"/>
-      <c r="X45" s="4"/>
-      <c r="Y45" s="4"/>
-      <c r="Z45" s="4"/>
-      <c r="AA45" s="4"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="5"/>
       <c r="AB45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="17" t="s">
+      <c r="A46" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="H46" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
-      <c r="U46" s="5"/>
-      <c r="V46" s="5"/>
-      <c r="W46" s="5"/>
-      <c r="X46" s="5"/>
-      <c r="Y46" s="5"/>
-      <c r="Z46" s="5"/>
-      <c r="AA46" s="5"/>
-      <c r="AB46" s="4"/>
     </row>
     <row r="47">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14" t="s">
+      <c r="B47" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5"/>
-      <c r="Y47" s="5"/>
-      <c r="Z47" s="5"/>
-      <c r="AA47" s="5"/>
-      <c r="AB47" s="4"/>
+      <c r="C47" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="G47" s="7"/>
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D48" s="7"/>
+      <c r="E48" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F48" s="21"/>
       <c r="H48" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D49" s="7"/>
-      <c r="G49" s="7"/>
+      <c r="E49" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="21" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F50" s="21"/>
       <c r="H50" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="F52" s="21"/>
-      <c r="H52" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="7" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D46:D47">
+    <dataValidation type="list" allowBlank="1" sqref="D44:D45">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2098,7 +2018,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2112,10 +2032,10 @@
         <v>73</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
@@ -2123,10 +2043,10 @@
         <v>73</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
@@ -2134,10 +2054,10 @@
         <v>73</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
@@ -2145,10 +2065,10 @@
         <v>73</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
@@ -2156,10 +2076,10 @@
         <v>73</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
@@ -2167,10 +2087,10 @@
         <v>73</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
@@ -2178,10 +2098,10 @@
         <v>73</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
@@ -2189,32 +2109,32 @@
         <v>73</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2237,47 +2157,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="22" t="s">
         <v>130</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C2" s="24" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-08-20_11-19</v>
+        <v>2023-09-21_09-35</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:including pahramacy pick-up appointment type
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
   <si>
     <t>type</t>
   </si>
@@ -278,7 +278,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>select_one appoint</t>
+    <t>select_one appoint or_other</t>
   </si>
   <si>
     <t>type_appoint</t>
@@ -290,7 +290,7 @@
     <t>welcome</t>
   </si>
   <si>
-    <t>Notes about this Appointment?</t>
+    <t>Notes about this Appointment</t>
   </si>
   <si>
     <t>select_one lab or_other</t>
@@ -375,6 +375,12 @@
   </si>
   <si>
     <t xml:space="preserve">External Referral </t>
+  </si>
+  <si>
+    <t>pharmacy</t>
+  </si>
+  <si>
+    <t>Pharmacy Pick-up Appointmen</t>
   </si>
   <si>
     <t>lab</t>
@@ -835,7 +841,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.75"/>
+    <col customWidth="1" min="1" max="1" width="24.75"/>
     <col customWidth="1" min="2" max="2" width="29.5"/>
     <col customWidth="1" min="3" max="3" width="62.13"/>
     <col customWidth="1" min="4" max="4" width="29.0"/>
@@ -2117,24 +2123,35 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>122</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2157,47 +2174,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C2" s="24" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-09-21_09-35</v>
+        <v>2024-04-16_11-32</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating reports for the level of care_test and appointment form
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="139">
   <si>
     <t>type</t>
   </si>
@@ -22,6 +22,9 @@
   </si>
   <si>
     <t>label</t>
+  </si>
+  <si>
+    <t>instance::tag</t>
   </si>
   <si>
     <t>media::image::en</t>
@@ -438,7 +441,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -470,6 +473,10 @@
       <sz val="11.0"/>
       <color rgb="FF833C0B"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="8.0"/>
@@ -538,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -575,6 +582,9 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -587,34 +597,34 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -843,14 +853,15 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="24.75"/>
     <col customWidth="1" min="2" max="2" width="29.5"/>
-    <col customWidth="1" min="3" max="3" width="62.13"/>
-    <col customWidth="1" min="4" max="4" width="29.0"/>
-    <col customWidth="1" min="5" max="5" width="36.75"/>
-    <col customWidth="1" min="6" max="6" width="11.88"/>
-    <col customWidth="1" min="7" max="7" width="42.13"/>
-    <col customWidth="1" min="8" max="8" width="15.25"/>
-    <col customWidth="1" min="9" max="9" width="22.63"/>
-    <col customWidth="1" min="11" max="11" width="19.63"/>
+    <col customWidth="1" min="3" max="3" width="35.5"/>
+    <col customWidth="1" min="4" max="4" width="23.38"/>
+    <col customWidth="1" min="5" max="5" width="29.0"/>
+    <col customWidth="1" min="6" max="6" width="36.75"/>
+    <col customWidth="1" min="7" max="7" width="11.88"/>
+    <col customWidth="1" min="8" max="8" width="42.13"/>
+    <col customWidth="1" min="9" max="9" width="15.25"/>
+    <col customWidth="1" min="10" max="10" width="22.63"/>
+    <col customWidth="1" min="12" max="12" width="19.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -866,13 +877,13 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -881,202 +892,214 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="10"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="4"/>
+      <c r="E10" s="10"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -1095,23 +1118,24 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -1130,23 +1154,24 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -1165,23 +1190,24 @@
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1200,24 +1226,25 @@
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
       <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -1236,242 +1263,264 @@
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
     </row>
     <row r="16">
       <c r="A16" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="E16" s="4"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17">
       <c r="A17" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" s="10"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" s="10"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="10"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="10"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
     </row>
     <row r="20">
       <c r="A20" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
     </row>
     <row r="21">
       <c r="A21" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22">
       <c r="A22" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
     </row>
     <row r="23">
       <c r="A23" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
     </row>
     <row r="24">
       <c r="A24" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" s="10"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="5" t="s">
-        <v>40</v>
+      <c r="I24" s="4"/>
+      <c r="J24" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D25" s="10"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="5" t="s">
-        <v>43</v>
+      <c r="I25" s="4"/>
+      <c r="J25" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4" t="s">
-        <v>45</v>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4" t="s">
-        <v>47</v>
+      <c r="G27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4" t="s">
-        <v>49</v>
+      <c r="G28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
@@ -1488,188 +1537,218 @@
       <c r="X29" s="4"/>
       <c r="Y29" s="4"/>
       <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4" t="s">
-        <v>53</v>
+      <c r="G30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="4"/>
+        <v>56</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4" t="s">
-        <v>56</v>
+      <c r="G31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4" t="s">
-        <v>58</v>
+      <c r="G32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4" t="s">
-        <v>60</v>
+      <c r="G33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="12" t="s">
-        <v>62</v>
+      <c r="G34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="13" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4" t="s">
-        <v>64</v>
+      <c r="G35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4" t="s">
-        <v>66</v>
+      <c r="G36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4" t="s">
-        <v>68</v>
+      <c r="G37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4" t="s">
-        <v>70</v>
+      <c r="G38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -1686,24 +1765,25 @@
       <c r="X39" s="4"/>
       <c r="Y39" s="4"/>
       <c r="Z39" s="4"/>
+      <c r="AA39" s="4"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>73</v>
+        <v>13</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="H40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -1724,22 +1804,25 @@
       <c r="Z40" s="4"/>
       <c r="AA40" s="4"/>
       <c r="AB40" s="4"/>
+      <c r="AC40" s="4"/>
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B41" s="15" t="s">
         <v>76</v>
       </c>
+      <c r="B41" s="16" t="s">
+        <v>77</v>
+      </c>
       <c r="C41" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="8"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -1760,18 +1843,21 @@
       <c r="Z41" s="4"/>
       <c r="AA41" s="4"/>
       <c r="AB41" s="4"/>
+      <c r="AC41" s="4"/>
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>79</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -1796,18 +1882,21 @@
       <c r="Z42" s="4"/>
       <c r="AA42" s="4"/>
       <c r="AB42" s="4"/>
+      <c r="AC42" s="4"/>
     </row>
     <row r="43">
       <c r="A43" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -1832,24 +1921,27 @@
       <c r="Z43" s="4"/>
       <c r="AA43" s="4"/>
       <c r="AB43" s="4"/>
+      <c r="AC43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>82</v>
+      <c r="A44" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>83</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="H44" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="15" t="s">
+        <v>84</v>
+      </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
@@ -1869,26 +1961,27 @@
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
       <c r="AA44" s="5"/>
-      <c r="AB44" s="4"/>
+      <c r="AB44" s="5"/>
+      <c r="AC44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>84</v>
+      <c r="A45" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>85</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="I45" s="5"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
@@ -1907,100 +2000,106 @@
       <c r="Y45" s="5"/>
       <c r="Z45" s="5"/>
       <c r="AA45" s="5"/>
-      <c r="AB45" s="4"/>
+      <c r="AB45" s="5"/>
+      <c r="AC45" s="4"/>
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="I46" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D46" s="7"/>
-      <c r="H46" s="7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D47" s="7"/>
-      <c r="G47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="H47" s="7"/>
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D48" s="7"/>
-      <c r="E48" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="F48" s="21"/>
-      <c r="H48" s="7" t="s">
-        <v>86</v>
+      <c r="E48" s="7"/>
+      <c r="F48" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G48" s="22"/>
+      <c r="I48" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D49" s="7"/>
-      <c r="E49" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>86</v>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="F50" s="21"/>
-      <c r="H50" s="7" t="s">
-        <v>86</v>
+      <c r="G50" s="22"/>
+      <c r="I50" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D44:D45">
+    <dataValidation type="list" allowBlank="1" sqref="E44:E45">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2024,7 +2123,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2035,123 +2134,123 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2174,47 +2273,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G1" s="22" t="s">
         <v>132</v>
       </c>
+      <c r="G1" s="23" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="24" t="str">
+      <c r="B2" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="25" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2024-04-16_11-32</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="25" t="s">
+        <v>2024-07-08_21-56</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>137</v>
+      </c>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates in the healthJam forms
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment.xlsx
+++ b/config/forms/app/appointment.xlsx
@@ -383,7 +383,7 @@
     <t>pharmacy</t>
   </si>
   <si>
-    <t>Pharmacy Pick-up Appointmen</t>
+    <t>Pharmacy Pick-up Appointment</t>
   </si>
   <si>
     <t>lab</t>
@@ -2303,7 +2303,7 @@
       </c>
       <c r="C2" s="25" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2024-07-08_21-56</v>
+        <v>2024-08-11_17-12</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>136</v>

</xml_diff>